<commit_message>
Adds metadata DB source loading and filling out associated json files from submission forms
</commit_message>
<xml_diff>
--- a/requests/ECHO_HIV_HI_PBMC_metadata.xlsx
+++ b/requests/ECHO_HIV_HI_PBMC_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MounSinai\Darpa\Programming\submission\requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB297AD9-DFEB-4317-B37D-6412F248321D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2E8CF0-8589-41D9-81FF-2658CCA0F3BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34230" yWindow="3105" windowWidth="17280" windowHeight="12225" xr2:uid="{1022EA94-C927-47D4-994A-3445E7764CD5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1022EA94-C927-47D4-994A-3445E7764CD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Submission_Request" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
   <si>
     <t>Project</t>
   </si>
@@ -601,7 +601,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648F6FB2-DCD5-4DC2-9468-8A496EE9201E}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
@@ -616,7 +616,7 @@
     <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -638,8 +638,14 @@
       <c r="G1" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -649,11 +655,8 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>57</v>
-      </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
         <v>64</v>
@@ -661,24 +664,36 @@
       <c r="G2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F5" s="1"/>
     </row>
   </sheetData>

</xml_diff>